<commit_message>
Versão 3.3 - adicionada matriz de correlação de critérios
</commit_message>
<xml_diff>
--- a/criterios_por_regiao.xlsx
+++ b/criterios_por_regiao.xlsx
@@ -517,49 +517,49 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1288888888888889</v>
+        <v>0.13</v>
       </c>
       <c r="C2" t="n">
-        <v>31.10111111111111</v>
+        <v>31.1</v>
       </c>
       <c r="D2" t="n">
-        <v>5.977777777777778</v>
+        <v>5.98</v>
       </c>
       <c r="E2" t="n">
-        <v>84.48222222222222</v>
+        <v>84.48</v>
       </c>
       <c r="F2" t="n">
-        <v>50.21555555555555</v>
+        <v>50.22</v>
       </c>
       <c r="G2" t="n">
-        <v>97.5911111111111</v>
+        <v>97.59</v>
       </c>
       <c r="H2" t="n">
-        <v>91.98444444444445</v>
+        <v>91.98</v>
       </c>
       <c r="I2" t="n">
-        <v>57.41333333333333</v>
+        <v>57.41</v>
       </c>
       <c r="J2" t="n">
-        <v>41.22111111111111</v>
+        <v>41.22</v>
       </c>
       <c r="K2" t="n">
-        <v>19.66888888888889</v>
+        <v>19.67</v>
       </c>
       <c r="L2" t="n">
-        <v>5.138888888888889</v>
+        <v>5.14</v>
       </c>
       <c r="M2" t="n">
-        <v>48.74333333333334</v>
+        <v>48.74</v>
       </c>
       <c r="N2" t="n">
-        <v>15.10666666666667</v>
+        <v>15.11</v>
       </c>
       <c r="O2" t="n">
-        <v>56.51888888888889</v>
+        <v>56.52</v>
       </c>
       <c r="P2" t="n">
-        <v>96.52777777777777</v>
+        <v>96.53</v>
       </c>
     </row>
     <row r="3">
@@ -572,46 +572,46 @@
         <v>0.08</v>
       </c>
       <c r="C3" t="n">
-        <v>35.30714285714286</v>
+        <v>35.31</v>
       </c>
       <c r="D3" t="n">
-        <v>6.351428571428572</v>
+        <v>6.35</v>
       </c>
       <c r="E3" t="n">
-        <v>83.30285714285715</v>
+        <v>83.3</v>
       </c>
       <c r="F3" t="n">
-        <v>58.17000000000001</v>
+        <v>58.17</v>
       </c>
       <c r="G3" t="n">
-        <v>95.34428571428573</v>
+        <v>95.34</v>
       </c>
       <c r="H3" t="n">
-        <v>88.96571428571428</v>
+        <v>88.97</v>
       </c>
       <c r="I3" t="n">
-        <v>52.73285714285714</v>
+        <v>52.73</v>
       </c>
       <c r="J3" t="n">
-        <v>45.15857142857143</v>
+        <v>45.16</v>
       </c>
       <c r="K3" t="n">
-        <v>18.90142857142857</v>
+        <v>18.9</v>
       </c>
       <c r="L3" t="n">
-        <v>6.300000000000002</v>
+        <v>6.3</v>
       </c>
       <c r="M3" t="n">
-        <v>57.08714285714285</v>
+        <v>57.09</v>
       </c>
       <c r="N3" t="n">
-        <v>13.50571428571429</v>
+        <v>13.51</v>
       </c>
       <c r="O3" t="n">
-        <v>56.52142857142857</v>
+        <v>56.52</v>
       </c>
       <c r="P3" t="n">
-        <v>96.90428571428572</v>
+        <v>96.90000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -621,7 +621,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5675</v>
+        <v>0.57</v>
       </c>
       <c r="C4" t="n">
         <v>42.66</v>
@@ -630,7 +630,7 @@
         <v>8.43</v>
       </c>
       <c r="E4" t="n">
-        <v>86.91249999999999</v>
+        <v>86.91</v>
       </c>
       <c r="F4" t="n">
         <v>54.8</v>
@@ -639,31 +639,31 @@
         <v>94.06999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>91.55000000000001</v>
+        <v>91.55</v>
       </c>
       <c r="I4" t="n">
-        <v>53.785</v>
+        <v>53.78</v>
       </c>
       <c r="J4" t="n">
-        <v>42.8725</v>
+        <v>42.87</v>
       </c>
       <c r="K4" t="n">
         <v>23.76</v>
       </c>
       <c r="L4" t="n">
-        <v>10.9925</v>
+        <v>10.99</v>
       </c>
       <c r="M4" t="n">
         <v>57.63</v>
       </c>
       <c r="N4" t="n">
-        <v>17.6875</v>
+        <v>17.69</v>
       </c>
       <c r="O4" t="n">
-        <v>54.03250000000001</v>
+        <v>54.03</v>
       </c>
       <c r="P4" t="n">
-        <v>97.77249999999999</v>
+        <v>97.77</v>
       </c>
     </row>
     <row r="5">
@@ -673,49 +673,49 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2625</v>
+        <v>0.26</v>
       </c>
       <c r="C5" t="n">
-        <v>41.145</v>
+        <v>41.14</v>
       </c>
       <c r="D5" t="n">
-        <v>4.8425</v>
+        <v>4.84</v>
       </c>
       <c r="E5" t="n">
-        <v>80.205</v>
+        <v>80.2</v>
       </c>
       <c r="F5" t="n">
-        <v>46.8475</v>
+        <v>46.85</v>
       </c>
       <c r="G5" t="n">
-        <v>97.3725</v>
+        <v>97.37</v>
       </c>
       <c r="H5" t="n">
         <v>86.37</v>
       </c>
       <c r="I5" t="n">
-        <v>59.415</v>
+        <v>59.42</v>
       </c>
       <c r="J5" t="n">
-        <v>35.5925</v>
+        <v>35.59</v>
       </c>
       <c r="K5" t="n">
         <v>14.09</v>
       </c>
       <c r="L5" t="n">
-        <v>5.095</v>
+        <v>5.1</v>
       </c>
       <c r="M5" t="n">
-        <v>54.8625</v>
+        <v>54.86</v>
       </c>
       <c r="N5" t="n">
-        <v>10.7375</v>
+        <v>10.74</v>
       </c>
       <c r="O5" t="n">
         <v>59.39</v>
       </c>
       <c r="P5" t="n">
-        <v>97.345</v>
+        <v>97.34</v>
       </c>
     </row>
     <row r="6">
@@ -725,34 +725,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1233333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="C6" t="n">
         <v>43.09</v>
       </c>
       <c r="D6" t="n">
-        <v>12.59333333333333</v>
+        <v>12.59</v>
       </c>
       <c r="E6" t="n">
-        <v>86.85666666666667</v>
+        <v>86.86</v>
       </c>
       <c r="F6" t="n">
-        <v>53.40666666666667</v>
+        <v>53.41</v>
       </c>
       <c r="G6" t="n">
-        <v>95.46666666666665</v>
+        <v>95.47</v>
       </c>
       <c r="H6" t="n">
-        <v>88.25999999999999</v>
+        <v>88.26000000000001</v>
       </c>
       <c r="I6" t="n">
-        <v>57.97666666666667</v>
+        <v>57.98</v>
       </c>
       <c r="J6" t="n">
-        <v>42.83666666666667</v>
+        <v>42.84</v>
       </c>
       <c r="K6" t="n">
-        <v>15.79333333333333</v>
+        <v>15.79</v>
       </c>
       <c r="L6" t="n">
         <v>3.9</v>
@@ -761,13 +761,13 @@
         <v>52.62</v>
       </c>
       <c r="N6" t="n">
-        <v>12.63666666666667</v>
+        <v>12.64</v>
       </c>
       <c r="O6" t="n">
         <v>57.27</v>
       </c>
       <c r="P6" t="n">
-        <v>98.78666666666668</v>
+        <v>98.79000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>